<commit_message>
Calculated statistics complete in excel file + changes to the program for the statistics
</commit_message>
<xml_diff>
--- a/corpusStatistics.xlsx
+++ b/corpusStatistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/github/Urdu_Fake_News/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37B839C-CAE5-6945-99A3-D02F679AFD58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9319945-B70B-464F-88A9-D91DA4F2F07B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13940" xr2:uid="{EA2BB066-887D-5345-B8E2-66447FF33CE3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{EA2BB066-887D-5345-B8E2-66447FF33CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -69,19 +69,22 @@
     <t>Overlap</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t>Vocabulary overlap within each category for Training Set</t>
   </si>
   <si>
     <t>Vocabulary overlap within each category for Testing Set</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -113,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -136,11 +139,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -165,6 +205,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D547085A-BE49-0547-903C-FA32576462BF}">
-  <dimension ref="B2:N20"/>
+  <dimension ref="B2:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E10" sqref="E10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +560,7 @@
     <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -499,17 +568,17 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="4" t="s">
         <v>5</v>
@@ -519,19 +588,19 @@
         <v>6</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="4"/>
+      <c r="M3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
@@ -547,312 +616,531 @@
       <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="H5" s="7" t="s">
+      <c r="C5" s="8">
+        <v>70</v>
+      </c>
+      <c r="D5" s="8">
+        <v>36</v>
+      </c>
+      <c r="E5" s="20">
+        <v>30</v>
+      </c>
+      <c r="F5" s="20">
+        <v>14</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="J5" s="8">
+        <v>4640</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1939</v>
+      </c>
+      <c r="L5" s="15">
+        <v>34.65</v>
+      </c>
+      <c r="M5" s="20">
+        <v>2822</v>
+      </c>
+      <c r="N5" s="20">
+        <v>862</v>
+      </c>
+      <c r="O5" s="20">
+        <v>25.690799999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="H6" s="7" t="s">
+      <c r="C6" s="8">
+        <v>70</v>
+      </c>
+      <c r="D6" s="8">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20">
+        <v>30</v>
+      </c>
+      <c r="F6" s="20">
+        <v>30</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="J6" s="8">
+        <v>3825</v>
+      </c>
+      <c r="K6" s="8">
+        <v>3454</v>
+      </c>
+      <c r="L6" s="8">
+        <v>55.633899999999997</v>
+      </c>
+      <c r="M6" s="20">
+        <v>2283</v>
+      </c>
+      <c r="N6" s="20">
+        <v>2091</v>
+      </c>
+      <c r="O6" s="20">
+        <v>72.408299999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="H7" s="7" t="s">
+      <c r="C7" s="8">
+        <v>70</v>
+      </c>
+      <c r="D7" s="8">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20">
+        <v>30</v>
+      </c>
+      <c r="F7" s="20">
+        <v>30</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="J7" s="8">
+        <v>3695</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3851</v>
+      </c>
+      <c r="L7" s="15">
+        <v>49.99</v>
+      </c>
+      <c r="M7" s="20">
+        <v>2919</v>
+      </c>
+      <c r="N7" s="20">
+        <v>2953</v>
+      </c>
+      <c r="O7" s="20">
+        <v>46.8367</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="H8" s="7" t="s">
+      <c r="C8" s="8">
+        <v>70</v>
+      </c>
+      <c r="D8" s="8">
+        <v>42</v>
+      </c>
+      <c r="E8" s="20">
+        <v>30</v>
+      </c>
+      <c r="F8" s="20">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="J8" s="8">
+        <v>4948</v>
+      </c>
+      <c r="K8" s="8">
+        <v>2178</v>
+      </c>
+      <c r="L8" s="8">
+        <v>34.5289</v>
+      </c>
+      <c r="M8" s="20">
+        <v>3365</v>
+      </c>
+      <c r="N8" s="20">
+        <v>536</v>
+      </c>
+      <c r="O8" s="21">
+        <v>13.930999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="H9" s="7" t="s">
+      <c r="C9" s="8">
+        <v>70</v>
+      </c>
+      <c r="D9" s="8">
+        <v>70</v>
+      </c>
+      <c r="E9" s="20">
+        <v>3</v>
+      </c>
+      <c r="F9" s="20">
+        <v>30</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="J9" s="8">
+        <v>4494</v>
+      </c>
+      <c r="K9" s="8">
+        <v>4679</v>
+      </c>
+      <c r="L9" s="8">
+        <v>56.535800000000002</v>
+      </c>
+      <c r="M9" s="20">
+        <v>2448</v>
+      </c>
+      <c r="N9" s="20">
+        <v>2458</v>
+      </c>
+      <c r="O9" s="20">
+        <v>56.491199999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <f>SUM(C5:C9)</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="8">
+        <v>350</v>
+      </c>
+      <c r="D10" s="6">
         <f t="shared" ref="D10:F10" si="0">SUM(D5:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
+        <v>288</v>
+      </c>
+      <c r="E10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="8">
+        <v>123</v>
+      </c>
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="6">
+        <v>13250</v>
+      </c>
+      <c r="K10" s="6">
+        <v>10115</v>
+      </c>
+      <c r="L10" s="19">
+        <v>47.375999999999998</v>
+      </c>
+      <c r="M10" s="6">
+        <v>8848</v>
+      </c>
+      <c r="N10" s="6">
+        <v>6110</v>
+      </c>
+      <c r="O10" s="6">
+        <v>45.1387</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="I14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H14" s="16"/>
+      <c r="I14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="H15" s="17"/>
       <c r="I15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N15" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="I16" s="7" t="s">
+      <c r="C16" s="9">
+        <v>100</v>
+      </c>
+      <c r="D16" s="9">
+        <v>24.615500000000001</v>
+      </c>
+      <c r="E16" s="9">
+        <v>22.4925</v>
+      </c>
+      <c r="F16" s="9">
+        <v>22.598099999999999</v>
+      </c>
+      <c r="G16" s="9">
+        <v>23.5456</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
+      <c r="J16" s="9">
+        <v>100</v>
+      </c>
+      <c r="K16" s="9">
+        <v>20.281500000000001</v>
+      </c>
+      <c r="L16" s="9">
+        <v>17.597100000000001</v>
+      </c>
+      <c r="M16" s="9">
+        <v>20.6798</v>
+      </c>
+      <c r="N16" s="9">
+        <v>23.267600000000002</v>
+      </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="I17" s="7" t="s">
+      <c r="C17" s="9">
+        <v>24.615500000000001</v>
+      </c>
+      <c r="D17" s="9">
+        <v>100</v>
+      </c>
+      <c r="E17" s="9">
+        <v>21.806699999999999</v>
+      </c>
+      <c r="F17" s="14">
+        <v>21.308599999999998</v>
+      </c>
+      <c r="G17" s="14">
+        <v>23.283000000000001</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
+      <c r="J17" s="9">
+        <v>20.281500000000001</v>
+      </c>
+      <c r="K17" s="9">
+        <v>100</v>
+      </c>
+      <c r="L17" s="9">
+        <v>16.195499999999999</v>
+      </c>
+      <c r="M17" s="14">
+        <v>18.556000000000001</v>
+      </c>
+      <c r="N17" s="9">
+        <v>21.795100000000001</v>
+      </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="I18" s="7" t="s">
+      <c r="C18" s="9">
+        <v>22.4925</v>
+      </c>
+      <c r="D18" s="9">
+        <v>21.806699999999999</v>
+      </c>
+      <c r="E18" s="9">
+        <v>100</v>
+      </c>
+      <c r="F18" s="14">
+        <v>21.121099999999998</v>
+      </c>
+      <c r="G18" s="9">
+        <v>20.010999999999999</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
+      <c r="J18" s="9">
+        <v>17.597100000000001</v>
+      </c>
+      <c r="K18" s="9">
+        <v>16.195499999999999</v>
+      </c>
+      <c r="L18" s="9">
+        <v>100</v>
+      </c>
+      <c r="M18" s="9">
+        <v>18.464700000000001</v>
+      </c>
+      <c r="N18" s="9">
+        <v>18.151700000000002</v>
+      </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="I19" s="7" t="s">
+      <c r="C19" s="9">
+        <v>22.598099999999999</v>
+      </c>
+      <c r="D19" s="14">
+        <v>21.308599999999998</v>
+      </c>
+      <c r="E19" s="14">
+        <v>21.121099999999998</v>
+      </c>
+      <c r="F19" s="9">
+        <v>100</v>
+      </c>
+      <c r="G19" s="9">
+        <v>19.300599999999999</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
+      <c r="J19" s="9">
+        <v>20.6798</v>
+      </c>
+      <c r="K19" s="14">
+        <v>18.556000000000001</v>
+      </c>
+      <c r="L19" s="9">
+        <v>18.464700000000001</v>
+      </c>
+      <c r="M19" s="9">
+        <v>100</v>
+      </c>
+      <c r="N19" s="9">
+        <v>20.106200000000001</v>
+      </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="I20" s="7" t="s">
+      <c r="C20" s="9">
+        <v>23.5456</v>
+      </c>
+      <c r="D20" s="14">
+        <v>23.283000000000001</v>
+      </c>
+      <c r="E20" s="14">
+        <v>20.010999999999999</v>
+      </c>
+      <c r="F20" s="9">
+        <v>19.300599999999999</v>
+      </c>
+      <c r="G20" s="9">
+        <v>100</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
+      <c r="J20" s="9">
+        <v>23.267600000000002</v>
+      </c>
+      <c r="K20" s="9">
+        <v>21.795100000000001</v>
+      </c>
+      <c r="L20" s="9">
+        <v>18.151700000000002</v>
+      </c>
+      <c r="M20" s="9">
+        <v>20.106200000000001</v>
+      </c>
+      <c r="N20" s="9">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -861,9 +1149,9 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="I2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Additional of finaL VERSIONS OF FILES
</commit_message>
<xml_diff>
--- a/corpusStatistics.xlsx
+++ b/corpusStatistics.xlsx
@@ -231,9 +231,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,6 +238,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1343,7 +1343,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24.615500000000001</c:v>
@@ -1423,7 +1423,7 @@
                   <c:v>24.615500000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>21.806699999999999</c:v>
@@ -1503,7 +1503,7 @@
                   <c:v>21.806699999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.0000">
                   <c:v>21.121099999999998</c:v>
@@ -1585,7 +1585,7 @@
                   <c:v>21.121099999999998</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>19.300599999999999</c:v>
@@ -1667,7 +1667,7 @@
                   <c:v>19.300599999999999</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3828,7 +3828,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4469,7 +4468,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7326,16 +7325,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>833436</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>441230</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>25214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>74519</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>25214</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7746,8 +7745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R52" sqref="R52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7758,24 +7757,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -7810,13 +7809,13 @@
       <c r="F5" s="16">
         <v>14</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
@@ -7835,14 +7834,14 @@
         <v>30</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20" t="s">
+      <c r="M6" s="23"/>
+      <c r="N6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="20"/>
+      <c r="O6" s="23"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
@@ -8042,14 +8041,14 @@
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
@@ -8076,7 +8075,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D30" s="8">
         <v>24.615500000000001</v>
@@ -8099,7 +8098,7 @@
         <v>24.615500000000001</v>
       </c>
       <c r="D31" s="8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E31" s="8">
         <v>21.806699999999999</v>
@@ -8122,7 +8121,7 @@
         <v>21.806699999999999</v>
       </c>
       <c r="E32" s="8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F32" s="10">
         <v>21.121099999999998</v>
@@ -8145,7 +8144,7 @@
         <v>21.121099999999998</v>
       </c>
       <c r="F33" s="8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G33" s="8">
         <v>19.300599999999999</v>
@@ -8168,15 +8167,15 @@
         <v>19.300599999999999</v>
       </c>
       <c r="G34" s="8">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="M35" s="21" t="s">
+      <c r="M35" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="N35" s="22"/>
-      <c r="O35" s="23"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="22"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M36" s="18"/>
@@ -8270,14 +8269,14 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="23"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="22"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
@@ -8407,15 +8406,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="M35:O35"/>
     <mergeCell ref="B64:G64"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="M35:O35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>